<commit_message>
Now makes a file, but only reads EOF Token
</commit_message>
<xml_diff>
--- a/Timelog.xlsx
+++ b/Timelog.xlsx
@@ -447,6 +447,14 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
@@ -469,14 +477,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -797,7 +797,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,26 +810,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8"/>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="19" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="21" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="10"/>
       <c r="C2" s="11" t="s">
         <v>3</v>
@@ -852,7 +852,7 @@
       <c r="I2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="20"/>
+      <c r="J2" s="22"/>
       <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="4.9000000000000004" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -869,7 +869,7 @@
       <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="25">
+      <c r="A4" s="19">
         <v>1</v>
       </c>
       <c r="B4" s="10"/>
@@ -901,7 +901,7 @@
       <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="10"/>
       <c r="C5" s="16">
         <f>IF(C4="", "", C4)</f>
@@ -938,29 +938,39 @@
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="25">
+      <c r="A6" s="19">
         <v>2</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="6"/>
       <c r="J6" s="15">
         <f>IF(C6="", 0, SUM(C6:I6))</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="16" t="str">
+      <c r="C7" s="16">
         <f>IF(C6="", "", J5+C6)</f>
-        <v/>
+        <v>8.5</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>10</v>
@@ -982,12 +992,12 @@
       </c>
       <c r="J7" s="18">
         <f>IF(C7="", J5, J5+J6)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
+      <c r="A8" s="19">
         <v>3</v>
       </c>
       <c r="B8" s="10"/>
@@ -1005,7 +1015,7 @@
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="10"/>
       <c r="C9" s="16" t="str">
         <f>IF(C8="", "", J7+C8)</f>
@@ -1031,12 +1041,12 @@
       </c>
       <c r="J9" s="18">
         <f>IF(C9="", J7, J7+J8)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="25">
+      <c r="A10" s="19">
         <v>4</v>
       </c>
       <c r="B10" s="10"/>
@@ -1054,7 +1064,7 @@
       <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="10"/>
       <c r="C11" s="16" t="str">
         <f>IF(C10="", "", J9+C10)</f>
@@ -1080,12 +1090,12 @@
       </c>
       <c r="J11" s="18">
         <f>IF(C11="", J9, J9+J10)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="25">
+      <c r="A12" s="19">
         <v>5</v>
       </c>
       <c r="B12" s="10"/>
@@ -1103,7 +1113,7 @@
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="10"/>
       <c r="C13" s="16" t="str">
         <f>IF(C12="", "", J11+C12)</f>
@@ -1129,12 +1139,12 @@
       </c>
       <c r="J13" s="18">
         <f>IF(C13="", J11, J11+J12)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="25">
+      <c r="A14" s="19">
         <v>6</v>
       </c>
       <c r="B14" s="10"/>
@@ -1152,7 +1162,7 @@
       <c r="K14" s="10"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="10"/>
       <c r="C15" s="16" t="str">
         <f>IF(C14="", "", J13+C14)</f>
@@ -1178,12 +1188,12 @@
       </c>
       <c r="J15" s="18">
         <f>IF(C15="", J13, J13+J14)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="25">
+      <c r="A16" s="19">
         <v>7</v>
       </c>
       <c r="B16" s="10"/>
@@ -1201,7 +1211,7 @@
       <c r="K16" s="10"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="10"/>
       <c r="C17" s="16" t="str">
         <f>IF(C16="", "", J15+C16)</f>
@@ -1227,12 +1237,12 @@
       </c>
       <c r="J17" s="18">
         <f>IF(C17="", J15, J15+J16)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="25">
+      <c r="A18" s="19">
         <v>8</v>
       </c>
       <c r="B18" s="10"/>
@@ -1250,7 +1260,7 @@
       <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="10"/>
       <c r="C19" s="16" t="str">
         <f>IF(C18="", "", J17+C18)</f>
@@ -1276,12 +1286,12 @@
       </c>
       <c r="J19" s="18">
         <f>IF(C19="", J17, J17+J18)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K19" s="10"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="25">
+      <c r="A20" s="19">
         <v>9</v>
       </c>
       <c r="B20" s="10"/>
@@ -1299,7 +1309,7 @@
       <c r="K20" s="10"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="10"/>
       <c r="C21" s="16" t="str">
         <f>IF(C20="", "", J19+C20)</f>
@@ -1325,12 +1335,12 @@
       </c>
       <c r="J21" s="18">
         <f>IF(C21="", J19, J19+J20)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K21" s="10"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="25">
+      <c r="A22" s="19">
         <v>10</v>
       </c>
       <c r="B22" s="10"/>
@@ -1348,7 +1358,7 @@
       <c r="K22" s="10"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="10"/>
       <c r="C23" s="16" t="str">
         <f>IF(C22="", "", J21+C22)</f>
@@ -1374,12 +1384,12 @@
       </c>
       <c r="J23" s="18">
         <f>IF(C23="", J21, J21+J22)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K23" s="10"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="25">
+      <c r="A24" s="19">
         <v>11</v>
       </c>
       <c r="B24" s="10"/>
@@ -1397,7 +1407,7 @@
       <c r="K24" s="10"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="10"/>
       <c r="C25" s="16" t="str">
         <f>IF(C24="", "", J23+C24)</f>
@@ -1423,12 +1433,12 @@
       </c>
       <c r="J25" s="18">
         <f>IF(C25="", J23, J23+J24)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K25" s="10"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="25">
+      <c r="A26" s="19">
         <v>12</v>
       </c>
       <c r="B26" s="10"/>
@@ -1446,7 +1456,7 @@
       <c r="K26" s="10"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="26"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="10"/>
       <c r="C27" s="16" t="str">
         <f>IF(C26="", "", J25+C26)</f>
@@ -1472,12 +1482,12 @@
       </c>
       <c r="J27" s="18">
         <f>IF(C27="", J25, J25+J26)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K27" s="10"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="25">
+      <c r="A28" s="19">
         <v>13</v>
       </c>
       <c r="B28" s="10"/>
@@ -1495,7 +1505,7 @@
       <c r="K28" s="10"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="26"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="10"/>
       <c r="C29" s="16" t="str">
         <f>IF(C28="", "", J27+C28)</f>
@@ -1521,12 +1531,12 @@
       </c>
       <c r="J29" s="18">
         <f>IF(C29="", J27, J27+J28)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K29" s="10"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="25">
+      <c r="A30" s="19">
         <v>14</v>
       </c>
       <c r="B30" s="10"/>
@@ -1544,7 +1554,7 @@
       <c r="K30" s="10"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="10"/>
       <c r="C31" s="16" t="str">
         <f>IF(C30="", "", J29+C30)</f>
@@ -1570,12 +1580,12 @@
       </c>
       <c r="J31" s="18">
         <f>IF(C31="", J29, J29+J30)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K31" s="10"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="25">
+      <c r="A32" s="19">
         <v>15</v>
       </c>
       <c r="B32" s="10"/>
@@ -1593,7 +1603,7 @@
       <c r="K32" s="10"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="26"/>
+      <c r="A33" s="20"/>
       <c r="B33" s="10"/>
       <c r="C33" s="16" t="str">
         <f>IF(C32="", "", J31+C32)</f>
@@ -1619,12 +1629,12 @@
       </c>
       <c r="J33" s="18">
         <f>IF(C33="", J31, J31+J32)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K33" s="10"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="25">
+      <c r="A34" s="19">
         <v>16</v>
       </c>
       <c r="B34" s="10"/>
@@ -1642,7 +1652,7 @@
       <c r="K34" s="10"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="26"/>
+      <c r="A35" s="20"/>
       <c r="B35" s="10"/>
       <c r="C35" s="16" t="str">
         <f>IF(C34="", "", J33+C34)</f>
@@ -1668,7 +1678,7 @@
       </c>
       <c r="J35" s="18">
         <f>IF(C35="", J33, J33+J34)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="K35" s="10"/>
     </row>
@@ -1688,6 +1698,16 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="19">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -1697,16 +1717,6 @@
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Can do some basic int operations, no order of ops
</commit_message>
<xml_diff>
--- a/Timelog.xlsx
+++ b/Timelog.xlsx
@@ -797,7 +797,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,17 +1195,21 @@
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
         <v>2</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2">
+        <v>2.5</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="7"/>
       <c r="J14" s="15">
         <f>IF(C14="", 0, SUM(C14:I14))</f>
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="K14" s="10"/>
     </row>
@@ -1214,7 +1218,7 @@
       <c r="B15" s="10"/>
       <c r="C15" s="16">
         <f>IF(C14="", "", J13+C14)</f>
-        <v>39.5</v>
+        <v>37.5</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>10</v>
@@ -1236,7 +1240,7 @@
       </c>
       <c r="J15" s="18">
         <f>IF(C15="", J13, J13+J14)</f>
-        <v>39.5</v>
+        <v>42</v>
       </c>
       <c r="K15" s="10"/>
     </row>
@@ -1285,7 +1289,7 @@
       </c>
       <c r="J17" s="18">
         <f>IF(C17="", J15, J15+J16)</f>
-        <v>39.5</v>
+        <v>42</v>
       </c>
       <c r="K17" s="10"/>
     </row>
@@ -1334,7 +1338,7 @@
       </c>
       <c r="J19" s="18">
         <f>IF(C19="", J17, J17+J18)</f>
-        <v>39.5</v>
+        <v>42</v>
       </c>
       <c r="K19" s="10"/>
     </row>
@@ -1383,7 +1387,7 @@
       </c>
       <c r="J21" s="18">
         <f>IF(C21="", J19, J19+J20)</f>
-        <v>39.5</v>
+        <v>42</v>
       </c>
       <c r="K21" s="10"/>
     </row>
@@ -1432,7 +1436,7 @@
       </c>
       <c r="J23" s="18">
         <f>IF(C23="", J21, J21+J22)</f>
-        <v>39.5</v>
+        <v>42</v>
       </c>
       <c r="K23" s="10"/>
     </row>
@@ -1481,7 +1485,7 @@
       </c>
       <c r="J25" s="18">
         <f>IF(C25="", J23, J23+J24)</f>
-        <v>39.5</v>
+        <v>42</v>
       </c>
       <c r="K25" s="10"/>
     </row>
@@ -1530,7 +1534,7 @@
       </c>
       <c r="J27" s="18">
         <f>IF(C27="", J25, J25+J26)</f>
-        <v>39.5</v>
+        <v>42</v>
       </c>
       <c r="K27" s="10"/>
     </row>
@@ -1579,7 +1583,7 @@
       </c>
       <c r="J29" s="18">
         <f>IF(C29="", J27, J27+J28)</f>
-        <v>39.5</v>
+        <v>42</v>
       </c>
       <c r="K29" s="10"/>
     </row>
@@ -1628,7 +1632,7 @@
       </c>
       <c r="J31" s="18">
         <f>IF(C31="", J29, J29+J30)</f>
-        <v>39.5</v>
+        <v>42</v>
       </c>
       <c r="K31" s="10"/>
     </row>
@@ -1677,7 +1681,7 @@
       </c>
       <c r="J33" s="18">
         <f>IF(C33="", J31, J31+J32)</f>
-        <v>39.5</v>
+        <v>42</v>
       </c>
       <c r="K33" s="10"/>
     </row>
@@ -1726,7 +1730,7 @@
       </c>
       <c r="J35" s="18">
         <f>IF(C35="", J33, J33+J34)</f>
-        <v>39.5</v>
+        <v>42</v>
       </c>
       <c r="K35" s="10"/>
     </row>

</xml_diff>

<commit_message>
Test 5 Works, Refactored
</commit_message>
<xml_diff>
--- a/Timelog.xlsx
+++ b/Timelog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -447,36 +447,36 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -797,7 +797,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,26 +810,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8"/>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="21" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="19" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
+      <c r="A2" s="22"/>
       <c r="B2" s="10"/>
       <c r="C2" s="11" t="s">
         <v>3</v>
@@ -852,7 +852,7 @@
       <c r="I2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="22"/>
+      <c r="J2" s="20"/>
       <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="4.9000000000000004" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -869,7 +869,7 @@
       <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+      <c r="A4" s="25">
         <v>1</v>
       </c>
       <c r="B4" s="10"/>
@@ -901,7 +901,7 @@
       <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="10"/>
       <c r="C5" s="16">
         <f>IF(C4="", "", C4)</f>
@@ -938,7 +938,7 @@
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
+      <c r="A6" s="25">
         <v>2</v>
       </c>
       <c r="B6" s="10"/>
@@ -970,7 +970,7 @@
       <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="10"/>
       <c r="C7" s="16">
         <f>IF(C6="", "", J5+C6)</f>
@@ -1001,7 +1001,7 @@
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
+      <c r="A8" s="25">
         <v>3</v>
       </c>
       <c r="B8" s="10"/>
@@ -1033,7 +1033,7 @@
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="10"/>
       <c r="C9" s="16">
         <f>IF(C8="", "", J7+C8)</f>
@@ -1064,7 +1064,7 @@
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+      <c r="A10" s="25">
         <v>4</v>
       </c>
       <c r="B10" s="10"/>
@@ -1096,7 +1096,7 @@
       <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="10"/>
       <c r="C11" s="16">
         <f>IF(C10="", "", J9+C10)</f>
@@ -1127,7 +1127,7 @@
       <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="A12" s="25">
         <v>5</v>
       </c>
       <c r="B12" s="10"/>
@@ -1159,7 +1159,7 @@
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="10"/>
       <c r="C13" s="16">
         <f>IF(C12="", "", J11+C12)</f>
@@ -1190,7 +1190,7 @@
       <c r="K13" s="10"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
+      <c r="A14" s="25">
         <v>6</v>
       </c>
       <c r="B14" s="10"/>
@@ -1203,18 +1203,26 @@
       <c r="E14" s="2">
         <v>2.5</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="7"/>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7">
+        <v>2</v>
+      </c>
       <c r="J14" s="15">
         <f>IF(C14="", 0, SUM(C14:I14))</f>
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="10"/>
       <c r="C15" s="16">
         <f>IF(C14="", "", J13+C14)</f>
@@ -1240,34 +1248,48 @@
       </c>
       <c r="J15" s="18">
         <f>IF(C15="", J13, J13+J14)</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
+      <c r="A16" s="25">
         <v>7</v>
       </c>
       <c r="B16" s="10"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="7"/>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0</v>
+      </c>
       <c r="J16" s="15">
         <f>IF(C16="", 0, SUM(C16:I16))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K16" s="10"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="16" t="str">
+      <c r="C17" s="16">
         <f>IF(C16="", "", J15+C16)</f>
-        <v/>
+        <v>46</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>10</v>
@@ -1289,34 +1311,48 @@
       </c>
       <c r="J17" s="18">
         <f>IF(C17="", J15, J15+J16)</f>
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="25">
         <v>8</v>
       </c>
       <c r="B18" s="10"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="7"/>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="7">
+        <v>0</v>
+      </c>
       <c r="J18" s="15">
         <f>IF(C18="", 0, SUM(C18:I18))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="10"/>
-      <c r="C19" s="16" t="str">
+      <c r="C19" s="16">
         <f>IF(C18="", "", J17+C18)</f>
-        <v/>
+        <v>50</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>10</v>
@@ -1338,34 +1374,46 @@
       </c>
       <c r="J19" s="18">
         <f>IF(C19="", J17, J17+J18)</f>
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="K19" s="10"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
+      <c r="A20" s="25">
         <v>9</v>
       </c>
       <c r="B20" s="10"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>3</v>
+      </c>
+      <c r="G20" s="2">
+        <v>3</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
       <c r="I20" s="7"/>
       <c r="J20" s="15">
         <f>IF(C20="", 0, SUM(C20:I20))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K20" s="10"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="16" t="str">
+      <c r="C21" s="16">
         <f>IF(C20="", "", J19+C20)</f>
-        <v/>
+        <v>51</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>10</v>
@@ -1387,12 +1435,12 @@
       </c>
       <c r="J21" s="18">
         <f>IF(C21="", J19, J19+J20)</f>
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="K21" s="10"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="19">
+      <c r="A22" s="25">
         <v>10</v>
       </c>
       <c r="B22" s="10"/>
@@ -1410,7 +1458,7 @@
       <c r="K22" s="10"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="10"/>
       <c r="C23" s="16" t="str">
         <f>IF(C22="", "", J21+C22)</f>
@@ -1436,12 +1484,12 @@
       </c>
       <c r="J23" s="18">
         <f>IF(C23="", J21, J21+J22)</f>
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="K23" s="10"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
+      <c r="A24" s="25">
         <v>11</v>
       </c>
       <c r="B24" s="10"/>
@@ -1459,7 +1507,7 @@
       <c r="K24" s="10"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="10"/>
       <c r="C25" s="16" t="str">
         <f>IF(C24="", "", J23+C24)</f>
@@ -1485,12 +1533,12 @@
       </c>
       <c r="J25" s="18">
         <f>IF(C25="", J23, J23+J24)</f>
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="K25" s="10"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="19">
+      <c r="A26" s="25">
         <v>12</v>
       </c>
       <c r="B26" s="10"/>
@@ -1508,7 +1556,7 @@
       <c r="K26" s="10"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="10"/>
       <c r="C27" s="16" t="str">
         <f>IF(C26="", "", J25+C26)</f>
@@ -1534,12 +1582,12 @@
       </c>
       <c r="J27" s="18">
         <f>IF(C27="", J25, J25+J26)</f>
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="K27" s="10"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="19">
+      <c r="A28" s="25">
         <v>13</v>
       </c>
       <c r="B28" s="10"/>
@@ -1557,7 +1605,7 @@
       <c r="K28" s="10"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="20"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="10"/>
       <c r="C29" s="16" t="str">
         <f>IF(C28="", "", J27+C28)</f>
@@ -1583,12 +1631,12 @@
       </c>
       <c r="J29" s="18">
         <f>IF(C29="", J27, J27+J28)</f>
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="K29" s="10"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="19">
+      <c r="A30" s="25">
         <v>14</v>
       </c>
       <c r="B30" s="10"/>
@@ -1606,7 +1654,7 @@
       <c r="K30" s="10"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="20"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="10"/>
       <c r="C31" s="16" t="str">
         <f>IF(C30="", "", J29+C30)</f>
@@ -1632,12 +1680,12 @@
       </c>
       <c r="J31" s="18">
         <f>IF(C31="", J29, J29+J30)</f>
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="K31" s="10"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="19">
+      <c r="A32" s="25">
         <v>15</v>
       </c>
       <c r="B32" s="10"/>
@@ -1655,7 +1703,7 @@
       <c r="K32" s="10"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="20"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="10"/>
       <c r="C33" s="16" t="str">
         <f>IF(C32="", "", J31+C32)</f>
@@ -1681,12 +1729,12 @@
       </c>
       <c r="J33" s="18">
         <f>IF(C33="", J31, J31+J32)</f>
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="K33" s="10"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="19">
+      <c r="A34" s="25">
         <v>16</v>
       </c>
       <c r="B34" s="10"/>
@@ -1704,7 +1752,7 @@
       <c r="K34" s="10"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="20"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="10"/>
       <c r="C35" s="16" t="str">
         <f>IF(C34="", "", J33+C34)</f>
@@ -1730,7 +1778,7 @@
       </c>
       <c r="J35" s="18">
         <f>IF(C35="", J33, J33+J34)</f>
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="K35" s="10"/>
     </row>
@@ -1750,16 +1798,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="19">
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -1769,6 +1807,16 @@
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Progress Made on Test 18
</commit_message>
<xml_diff>
--- a/Timelog.xlsx
+++ b/Timelog.xlsx
@@ -447,36 +447,36 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -797,7 +797,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,26 +810,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8"/>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="21" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="19" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
+      <c r="A2" s="22"/>
       <c r="B2" s="10"/>
       <c r="C2" s="11" t="s">
         <v>3</v>
@@ -852,7 +852,7 @@
       <c r="I2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="22"/>
+      <c r="J2" s="20"/>
       <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="4.9000000000000004" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -869,7 +869,7 @@
       <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+      <c r="A4" s="25">
         <v>1</v>
       </c>
       <c r="B4" s="10"/>
@@ -901,7 +901,7 @@
       <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="10"/>
       <c r="C5" s="16">
         <f>IF(C4="", "", C4)</f>
@@ -938,7 +938,7 @@
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
+      <c r="A6" s="25">
         <v>2</v>
       </c>
       <c r="B6" s="10"/>
@@ -970,7 +970,7 @@
       <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="10"/>
       <c r="C7" s="16">
         <f>IF(C6="", "", J5+C6)</f>
@@ -1001,7 +1001,7 @@
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
+      <c r="A8" s="25">
         <v>3</v>
       </c>
       <c r="B8" s="10"/>
@@ -1033,7 +1033,7 @@
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="10"/>
       <c r="C9" s="16">
         <f>IF(C8="", "", J7+C8)</f>
@@ -1064,7 +1064,7 @@
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+      <c r="A10" s="25">
         <v>4</v>
       </c>
       <c r="B10" s="10"/>
@@ -1096,7 +1096,7 @@
       <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="10"/>
       <c r="C11" s="16">
         <f>IF(C10="", "", J9+C10)</f>
@@ -1127,7 +1127,7 @@
       <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="A12" s="25">
         <v>5</v>
       </c>
       <c r="B12" s="10"/>
@@ -1159,7 +1159,7 @@
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="10"/>
       <c r="C13" s="16">
         <f>IF(C12="", "", J11+C12)</f>
@@ -1190,7 +1190,7 @@
       <c r="K13" s="10"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
+      <c r="A14" s="25">
         <v>6</v>
       </c>
       <c r="B14" s="10"/>
@@ -1222,7 +1222,7 @@
       <c r="K14" s="10"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="10"/>
       <c r="C15" s="16">
         <f>IF(C14="", "", J13+C14)</f>
@@ -1253,7 +1253,7 @@
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
+      <c r="A16" s="25">
         <v>7</v>
       </c>
       <c r="B16" s="10"/>
@@ -1285,7 +1285,7 @@
       <c r="K16" s="10"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="10"/>
       <c r="C17" s="16">
         <f>IF(C16="", "", J15+C16)</f>
@@ -1316,7 +1316,7 @@
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="25">
         <v>8</v>
       </c>
       <c r="B18" s="10"/>
@@ -1348,7 +1348,7 @@
       <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="10"/>
       <c r="C19" s="16">
         <f>IF(C18="", "", J17+C18)</f>
@@ -1379,7 +1379,7 @@
       <c r="K19" s="10"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
+      <c r="A20" s="25">
         <v>9</v>
       </c>
       <c r="B20" s="10"/>
@@ -1411,7 +1411,7 @@
       <c r="K20" s="10"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="10"/>
       <c r="C21" s="16">
         <f>IF(C20="", "", J19+C20)</f>
@@ -1442,7 +1442,7 @@
       <c r="K21" s="10"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="19">
+      <c r="A22" s="25">
         <v>10</v>
       </c>
       <c r="B22" s="10"/>
@@ -1474,7 +1474,7 @@
       <c r="K22" s="10"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="10"/>
       <c r="C23" s="16">
         <f>IF(C22="", "", J21+C22)</f>
@@ -1505,7 +1505,7 @@
       <c r="K23" s="10"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
+      <c r="A24" s="25">
         <v>11</v>
       </c>
       <c r="B24" s="10"/>
@@ -1537,7 +1537,7 @@
       <c r="K24" s="10"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="10"/>
       <c r="C25" s="16">
         <f>IF(C24="", "", J23+C24)</f>
@@ -1568,7 +1568,7 @@
       <c r="K25" s="10"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="19">
+      <c r="A26" s="25">
         <v>12</v>
       </c>
       <c r="B26" s="10"/>
@@ -1600,7 +1600,7 @@
       <c r="K26" s="10"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="10"/>
       <c r="C27" s="16">
         <f>IF(C26="", "", J25+C26)</f>
@@ -1631,7 +1631,7 @@
       <c r="K27" s="10"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="19">
+      <c r="A28" s="25">
         <v>13</v>
       </c>
       <c r="B28" s="10"/>
@@ -1663,7 +1663,7 @@
       <c r="K28" s="10"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="20"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="10"/>
       <c r="C29" s="16">
         <f>IF(C28="", "", J27+C28)</f>
@@ -1694,7 +1694,7 @@
       <c r="K29" s="10"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="19">
+      <c r="A30" s="25">
         <v>14</v>
       </c>
       <c r="B30" s="10"/>
@@ -1726,7 +1726,7 @@
       <c r="K30" s="10"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="20"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="10"/>
       <c r="C31" s="16">
         <f>IF(C30="", "", J29+C30)</f>
@@ -1757,7 +1757,7 @@
       <c r="K31" s="10"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="19">
+      <c r="A32" s="25">
         <v>15</v>
       </c>
       <c r="B32" s="10"/>
@@ -1770,18 +1770,24 @@
       <c r="E32" s="2">
         <v>3.5</v>
       </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1</v>
+      </c>
       <c r="I32" s="3"/>
       <c r="J32" s="15">
         <f>IF(C32="", 0, SUM(C32:I32))</f>
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
       <c r="K32" s="10"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="20"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="10"/>
       <c r="C33" s="16">
         <f>IF(C32="", "", J31+C32)</f>
@@ -1807,12 +1813,12 @@
       </c>
       <c r="J33" s="18">
         <f>IF(C33="", J31, J31+J32)</f>
-        <v>93.5</v>
+        <v>95.5</v>
       </c>
       <c r="K33" s="10"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="19">
+      <c r="A34" s="25">
         <v>16</v>
       </c>
       <c r="B34" s="10"/>
@@ -1830,7 +1836,7 @@
       <c r="K34" s="10"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="20"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="10"/>
       <c r="C35" s="16" t="str">
         <f>IF(C34="", "", J33+C34)</f>
@@ -1856,7 +1862,7 @@
       </c>
       <c r="J35" s="18">
         <f>IF(C35="", J33, J33+J34)</f>
-        <v>93.5</v>
+        <v>95.5</v>
       </c>
       <c r="K35" s="10"/>
     </row>
@@ -1876,16 +1882,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="19">
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -1895,6 +1891,16 @@
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Test 20 Works, Final Touches Made
</commit_message>
<xml_diff>
--- a/Timelog.xlsx
+++ b/Timelog.xlsx
@@ -447,6 +447,14 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
@@ -469,14 +477,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -797,7 +797,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,26 +810,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8"/>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="19" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="21" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="10"/>
       <c r="C2" s="11" t="s">
         <v>3</v>
@@ -852,7 +852,7 @@
       <c r="I2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="20"/>
+      <c r="J2" s="22"/>
       <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="4.9000000000000004" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -869,7 +869,7 @@
       <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="25">
+      <c r="A4" s="19">
         <v>1</v>
       </c>
       <c r="B4" s="10"/>
@@ -901,7 +901,7 @@
       <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="10"/>
       <c r="C5" s="16">
         <f>IF(C4="", "", C4)</f>
@@ -938,7 +938,7 @@
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="25">
+      <c r="A6" s="19">
         <v>2</v>
       </c>
       <c r="B6" s="10"/>
@@ -970,7 +970,7 @@
       <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="10"/>
       <c r="C7" s="16">
         <f>IF(C6="", "", J5+C6)</f>
@@ -1001,7 +1001,7 @@
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
+      <c r="A8" s="19">
         <v>3</v>
       </c>
       <c r="B8" s="10"/>
@@ -1033,7 +1033,7 @@
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="10"/>
       <c r="C9" s="16">
         <f>IF(C8="", "", J7+C8)</f>
@@ -1064,7 +1064,7 @@
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="25">
+      <c r="A10" s="19">
         <v>4</v>
       </c>
       <c r="B10" s="10"/>
@@ -1096,7 +1096,7 @@
       <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="10"/>
       <c r="C11" s="16">
         <f>IF(C10="", "", J9+C10)</f>
@@ -1127,7 +1127,7 @@
       <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="25">
+      <c r="A12" s="19">
         <v>5</v>
       </c>
       <c r="B12" s="10"/>
@@ -1159,7 +1159,7 @@
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="10"/>
       <c r="C13" s="16">
         <f>IF(C12="", "", J11+C12)</f>
@@ -1190,7 +1190,7 @@
       <c r="K13" s="10"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="25">
+      <c r="A14" s="19">
         <v>6</v>
       </c>
       <c r="B14" s="10"/>
@@ -1222,7 +1222,7 @@
       <c r="K14" s="10"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="10"/>
       <c r="C15" s="16">
         <f>IF(C14="", "", J13+C14)</f>
@@ -1253,7 +1253,7 @@
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="25">
+      <c r="A16" s="19">
         <v>7</v>
       </c>
       <c r="B16" s="10"/>
@@ -1285,7 +1285,7 @@
       <c r="K16" s="10"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="10"/>
       <c r="C17" s="16">
         <f>IF(C16="", "", J15+C16)</f>
@@ -1316,7 +1316,7 @@
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="25">
+      <c r="A18" s="19">
         <v>8</v>
       </c>
       <c r="B18" s="10"/>
@@ -1348,7 +1348,7 @@
       <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="10"/>
       <c r="C19" s="16">
         <f>IF(C18="", "", J17+C18)</f>
@@ -1379,7 +1379,7 @@
       <c r="K19" s="10"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="25">
+      <c r="A20" s="19">
         <v>9</v>
       </c>
       <c r="B20" s="10"/>
@@ -1411,7 +1411,7 @@
       <c r="K20" s="10"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="10"/>
       <c r="C21" s="16">
         <f>IF(C20="", "", J19+C20)</f>
@@ -1442,7 +1442,7 @@
       <c r="K21" s="10"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="25">
+      <c r="A22" s="19">
         <v>10</v>
       </c>
       <c r="B22" s="10"/>
@@ -1474,7 +1474,7 @@
       <c r="K22" s="10"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="10"/>
       <c r="C23" s="16">
         <f>IF(C22="", "", J21+C22)</f>
@@ -1505,7 +1505,7 @@
       <c r="K23" s="10"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="25">
+      <c r="A24" s="19">
         <v>11</v>
       </c>
       <c r="B24" s="10"/>
@@ -1537,7 +1537,7 @@
       <c r="K24" s="10"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="10"/>
       <c r="C25" s="16">
         <f>IF(C24="", "", J23+C24)</f>
@@ -1568,7 +1568,7 @@
       <c r="K25" s="10"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="25">
+      <c r="A26" s="19">
         <v>12</v>
       </c>
       <c r="B26" s="10"/>
@@ -1600,7 +1600,7 @@
       <c r="K26" s="10"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="26"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="10"/>
       <c r="C27" s="16">
         <f>IF(C26="", "", J25+C26)</f>
@@ -1631,7 +1631,7 @@
       <c r="K27" s="10"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="25">
+      <c r="A28" s="19">
         <v>13</v>
       </c>
       <c r="B28" s="10"/>
@@ -1663,7 +1663,7 @@
       <c r="K28" s="10"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="26"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="10"/>
       <c r="C29" s="16">
         <f>IF(C28="", "", J27+C28)</f>
@@ -1694,7 +1694,7 @@
       <c r="K29" s="10"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="25">
+      <c r="A30" s="19">
         <v>14</v>
       </c>
       <c r="B30" s="10"/>
@@ -1726,7 +1726,7 @@
       <c r="K30" s="10"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="10"/>
       <c r="C31" s="16">
         <f>IF(C30="", "", J29+C30)</f>
@@ -1757,7 +1757,7 @@
       <c r="K31" s="10"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="25">
+      <c r="A32" s="19">
         <v>15</v>
       </c>
       <c r="B32" s="10"/>
@@ -1777,17 +1777,19 @@
         <v>0</v>
       </c>
       <c r="H32" s="2">
-        <v>1</v>
-      </c>
-      <c r="I32" s="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="I32" s="3">
+        <v>5.5</v>
+      </c>
       <c r="J32" s="15">
         <f>IF(C32="", 0, SUM(C32:I32))</f>
-        <v>12.5</v>
+        <v>19.5</v>
       </c>
       <c r="K32" s="10"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="26"/>
+      <c r="A33" s="20"/>
       <c r="B33" s="10"/>
       <c r="C33" s="16">
         <f>IF(C32="", "", J31+C32)</f>
@@ -1813,16 +1815,18 @@
       </c>
       <c r="J33" s="18">
         <f>IF(C33="", J31, J31+J32)</f>
-        <v>95.5</v>
+        <v>102.5</v>
       </c>
       <c r="K33" s="10"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="25">
+      <c r="A34" s="19">
         <v>16</v>
       </c>
       <c r="B34" s="10"/>
-      <c r="C34" s="1"/>
+      <c r="C34" s="1">
+        <v>2</v>
+      </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -1831,16 +1835,16 @@
       <c r="I34" s="3"/>
       <c r="J34" s="15">
         <f>IF(C34="", 0, SUM(C34:I34))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K34" s="10"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="26"/>
+      <c r="A35" s="20"/>
       <c r="B35" s="10"/>
-      <c r="C35" s="16" t="str">
+      <c r="C35" s="16">
         <f>IF(C34="", "", J33+C34)</f>
-        <v/>
+        <v>104.5</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>10</v>
@@ -1862,7 +1866,7 @@
       </c>
       <c r="J35" s="18">
         <f>IF(C35="", J33, J33+J34)</f>
-        <v>95.5</v>
+        <v>104.5</v>
       </c>
       <c r="K35" s="10"/>
     </row>
@@ -1882,6 +1886,16 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="19">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -1891,16 +1905,6 @@
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>